<commit_message>
Signed-off-by: Jeff Robbins <JRS@qlik.com>
</commit_message>
<xml_diff>
--- a/External Data/XLS/Displayed Currencies.xlsx
+++ b/External Data/XLS/Displayed Currencies.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF108A42-0DF1-4302-A28E-74B05F44BEA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30ED0DEE-7400-42D1-8860-915B78B413A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,10 +99,10 @@
     <t>R$</t>
   </si>
   <si>
-    <t>BRA</t>
-  </si>
-  <si>
     <t>MXN</t>
+  </si>
+  <si>
+    <t>BRL</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,7 +561,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
         <v>23</v>
@@ -569,7 +569,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>16</v>

</xml_diff>